<commit_message>
Updated SAU model - 2025-08-21 12:54
</commit_message>
<xml_diff>
--- a/VerveStacks_SAU/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_SAU/SuppXLS/Scen_Base_VS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_SAU\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CDBFAED-A2B6-4663-AEF4-C62C7FC282F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C274DF70-31D3-4C9F-8CB6-511037661A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="12683" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Veda" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D257E54A-9E30-0669-8CC9-8DD8AE25BB01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2866233D-4B99-14E7-5449-732A1671B68E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>